<commit_message>
UPDATED ALL SS COURSES
SS courses are now lec lab separated with new numbers from excel sheet SS COURSES.xlsx
</commit_message>
<xml_diff>
--- a/BO Done.xlsx
+++ b/BO Done.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1168" sheetId="1" r:id="rId1"/>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,7 +1383,7 @@
         <v>38</v>
       </c>
       <c r="F19" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G19" s="8">
         <v>1</v>
@@ -1425,7 +1425,7 @@
         <v>38</v>
       </c>
       <c r="F20" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G20" s="8">
         <v>1</v>
@@ -1467,7 +1467,7 @@
         <v>38</v>
       </c>
       <c r="F21" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G21" s="8">
         <v>1</v>
@@ -1509,7 +1509,7 @@
         <v>38</v>
       </c>
       <c r="F22" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G22" s="8">
         <v>1</v>
@@ -1551,7 +1551,7 @@
         <v>38</v>
       </c>
       <c r="F23" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G23" s="8">
         <v>1</v>
@@ -1593,7 +1593,7 @@
         <v>38</v>
       </c>
       <c r="F24" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G24" s="8">
         <v>1</v>
@@ -1635,7 +1635,7 @@
         <v>38</v>
       </c>
       <c r="F25" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G25" s="8">
         <v>1</v>
@@ -1677,7 +1677,7 @@
         <v>38</v>
       </c>
       <c r="F26" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G26" s="8">
         <v>1</v>
@@ -1719,7 +1719,7 @@
         <v>38</v>
       </c>
       <c r="F27" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G27" s="8">
         <v>1</v>
@@ -2837,46 +2837,46 @@
       <c r="N53" s="10"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="7">
-        <v>1168</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" s="8" t="s">
+      <c r="A54" s="11">
+        <v>1168</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D54" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E54" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F54" s="8">
+      <c r="F54" s="12">
         <v>1520</v>
       </c>
-      <c r="G54" s="8">
-        <v>1</v>
-      </c>
-      <c r="H54" s="8">
-        <v>1</v>
-      </c>
-      <c r="I54" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J54" s="8" t="s">
+      <c r="G54" s="12">
+        <v>1</v>
+      </c>
+      <c r="H54" s="12">
+        <v>1</v>
+      </c>
+      <c r="I54" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="K54" s="8" t="s">
+      <c r="K54" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="L54" s="9">
+      <c r="L54" s="13">
         <v>0.60416666666666663</v>
       </c>
-      <c r="M54" s="9">
+      <c r="M54" s="13">
         <v>0.64583333333333337</v>
       </c>
-      <c r="N54" s="10"/>
+      <c r="N54" s="14"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
@@ -3853,8 +3853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4367,7 +4367,7 @@
         <v>38</v>
       </c>
       <c r="F13" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G13" s="8">
         <v>1</v>
@@ -4376,7 +4376,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>29</v>
@@ -4409,7 +4409,7 @@
         <v>38</v>
       </c>
       <c r="F14" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G14" s="8">
         <v>1</v>
@@ -4418,7 +4418,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>29</v>
@@ -4451,7 +4451,7 @@
         <v>38</v>
       </c>
       <c r="F15" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G15" s="8">
         <v>1</v>
@@ -4460,7 +4460,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>29</v>
@@ -4493,7 +4493,7 @@
         <v>38</v>
       </c>
       <c r="F16" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G16" s="8">
         <v>1</v>
@@ -4502,7 +4502,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>29</v>
@@ -4535,7 +4535,7 @@
         <v>38</v>
       </c>
       <c r="F17" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G17" s="8">
         <v>1</v>
@@ -4544,7 +4544,7 @@
         <v>1</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>29</v>
@@ -4577,7 +4577,7 @@
         <v>38</v>
       </c>
       <c r="F18" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G18" s="8">
         <v>1</v>
@@ -4586,7 +4586,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>29</v>
@@ -4619,7 +4619,7 @@
         <v>38</v>
       </c>
       <c r="F19" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G19" s="8">
         <v>1</v>
@@ -4628,7 +4628,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>29</v>
@@ -4661,7 +4661,7 @@
         <v>38</v>
       </c>
       <c r="F20" s="8">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="G20" s="8">
         <v>1</v>
@@ -4670,7 +4670,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J20" s="8" t="s">
         <v>29</v>
@@ -5039,7 +5039,7 @@
         <v>38</v>
       </c>
       <c r="F29" s="4">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="G29" s="4">
         <v>1</v>
@@ -5048,7 +5048,7 @@
         <v>1</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>35</v>
@@ -5081,7 +5081,7 @@
         <v>38</v>
       </c>
       <c r="F30" s="8">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="G30" s="8">
         <v>1</v>
@@ -5090,7 +5090,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J30" s="8" t="s">
         <v>35</v>
@@ -5123,7 +5123,7 @@
         <v>38</v>
       </c>
       <c r="F31" s="8">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="G31" s="8">
         <v>1</v>
@@ -5132,7 +5132,7 @@
         <v>1</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J31" s="8" t="s">
         <v>35</v>
@@ -5165,7 +5165,7 @@
         <v>38</v>
       </c>
       <c r="F32" s="8">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="G32" s="8">
         <v>1</v>
@@ -5174,7 +5174,7 @@
         <v>1</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J32" s="8" t="s">
         <v>35</v>
@@ -5207,7 +5207,7 @@
         <v>38</v>
       </c>
       <c r="F33" s="8">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="G33" s="8">
         <v>1</v>
@@ -5216,7 +5216,7 @@
         <v>1</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J33" s="8" t="s">
         <v>35</v>
@@ -5249,7 +5249,7 @@
         <v>38</v>
       </c>
       <c r="F34" s="8">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="G34" s="8">
         <v>1</v>
@@ -5258,7 +5258,7 @@
         <v>1</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J34" s="8" t="s">
         <v>35</v>
@@ -5291,7 +5291,7 @@
         <v>38</v>
       </c>
       <c r="F35" s="8">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="G35" s="8">
         <v>1</v>
@@ -5300,7 +5300,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="J35" s="8" t="s">
         <v>35</v>

</xml_diff>